<commit_message>
Updated BOM file links
</commit_message>
<xml_diff>
--- a/Documentation/OpenAT_Switch_Latch_BOM_v1.0.xlsx
+++ b/Documentation/OpenAT_Switch_Latch_BOM_v1.0.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26124"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26026"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://neilsquiresoc.sharepoint.com/sites/MMC-RD/Shared Documents/RD 22-09 Toggle Switch/OpenAT-Switch-Latch/Documentation/Working_Documents/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://neilsquiresoc.sharepoint.com/sites/MMC-RD/Shared Documents/RD 22-09 OpenAT Switch Latch/OpenAT-Switch-Latch/Documentation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="349" documentId="13_ncr:1_{0B8E08CA-0295-4D81-99D4-E8041F22A9F7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{02C43F76-176C-41C8-BDC8-81E874A7E493}"/>
+  <xr:revisionPtr revIDLastSave="352" documentId="13_ncr:1_{0B8E08CA-0295-4D81-99D4-E8041F22A9F7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{80CFE1A9-5838-48D6-9888-8DBA7596E21D}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1560" yWindow="720" windowWidth="12900" windowHeight="10200" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="OpenAT Switch Latch BOM V1.0" sheetId="2" r:id="rId1"/>
@@ -160,9 +160,6 @@
     <t>R3</t>
   </si>
   <si>
-    <t xml:space="preserve"> </t>
-  </si>
-  <si>
     <t>0.1 µF ±10% Capacitor</t>
   </si>
   <si>
@@ -296,6 +293,9 @@
   </si>
   <si>
     <t>https://www.digikey.ca/en/products/detail/b-f-fastener-supply/PSMS-004-0038-PH/333049</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> https://www.digikey.ca/en/products/detail/stackpole-electronics-inc/CFM14JT10K0/1742061</t>
   </si>
 </sst>
 </file>
@@ -303,10 +303,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
-    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="164" formatCode="_-&quot;$&quot;* #,##0.00_-;\-&quot;$&quot;* #,##0.00_-;_-&quot;$&quot;* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="44" formatCode="_-&quot;$&quot;* #,##0.00_-;\-&quot;$&quot;* #,##0.00_-;_-&quot;$&quot;* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="164" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
-  <fonts count="11">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -570,7 +570,7 @@
   </borders>
   <cellStyleXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -582,37 +582,37 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="2" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="3" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="4" applyFont="1"/>
-    <xf numFmtId="44" fontId="4" fillId="2" borderId="0" xfId="2" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="0" xfId="2" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="4"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="5"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="7" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="6" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="44" fontId="0" fillId="6" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="164" fontId="0" fillId="7" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="44" fontId="0" fillId="7" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="10" fillId="3" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="5" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="8" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="6" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="44" fontId="0" fillId="8" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="44" fontId="0" fillId="6" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="5" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="6" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="3" fillId="6" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="44" fontId="3" fillId="6" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="20" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
@@ -902,11 +902,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{25228E77-4763-43C3-812A-33F72B26FF01}">
   <dimension ref="A1:M43"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+    <sheetView tabSelected="1" topLeftCell="H2" workbookViewId="0">
+      <selection activeCell="J10" sqref="J10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="47.140625" customWidth="1"/>
     <col min="2" max="2" width="37.28515625" bestFit="1" customWidth="1"/>
@@ -922,7 +922,7 @@
     <col min="13" max="13" width="89.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="34.5">
+    <row r="1" spans="1:12" ht="34.5" x14ac:dyDescent="0.45">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -936,7 +936,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:12" ht="19.5" thickBot="1">
+    <row r="2" spans="1:12" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A2" s="13" t="s">
         <v>4</v>
       </c>
@@ -957,12 +957,12 @@
         <v>27.3</v>
       </c>
     </row>
-    <row r="3" spans="1:12" ht="16.5" thickBot="1">
+    <row r="3" spans="1:12" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="14" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:12" ht="15.75" thickBot="1">
+    <row r="4" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="15" t="s">
         <v>7</v>
       </c>
@@ -998,7 +998,7 @@
       </c>
       <c r="L4" s="7"/>
     </row>
-    <row r="5" spans="1:12">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" s="23" t="s">
         <v>18</v>
       </c>
@@ -1029,7 +1029,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="6" spans="1:12">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" s="23" t="s">
         <v>18</v>
       </c>
@@ -1060,7 +1060,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="7" spans="1:12">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" s="23" t="s">
         <v>18</v>
       </c>
@@ -1091,7 +1091,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="8" spans="1:12">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8" s="23" t="s">
         <v>18</v>
       </c>
@@ -1122,7 +1122,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="9" spans="1:12">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9" s="23" t="s">
         <v>18</v>
       </c>
@@ -1153,7 +1153,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="10" spans="1:12">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10" s="23" t="s">
         <v>18</v>
       </c>
@@ -1181,18 +1181,18 @@
         <v>0.16</v>
       </c>
       <c r="J10" s="25" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="11" spans="1:12">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A11" s="23" t="s">
         <v>18</v>
       </c>
       <c r="B11" s="23" t="s">
+        <v>36</v>
+      </c>
+      <c r="C11" s="23" t="s">
         <v>37</v>
-      </c>
-      <c r="C11" s="23" t="s">
-        <v>38</v>
       </c>
       <c r="D11" s="23">
         <v>1</v>
@@ -1212,18 +1212,18 @@
         <v>0.31</v>
       </c>
       <c r="J11" s="25" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="12" spans="1:12">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A12" s="23" t="s">
         <v>18</v>
       </c>
       <c r="B12" s="23" t="s">
+        <v>39</v>
+      </c>
+      <c r="C12" s="23" t="s">
         <v>40</v>
-      </c>
-      <c r="C12" s="23" t="s">
-        <v>41</v>
       </c>
       <c r="D12" s="23">
         <v>1</v>
@@ -1243,18 +1243,18 @@
         <v>1.18</v>
       </c>
       <c r="J12" s="25" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="13" spans="1:12">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A13" s="23" t="s">
         <v>18</v>
       </c>
       <c r="B13" s="23" t="s">
+        <v>42</v>
+      </c>
+      <c r="C13" s="23" t="s">
         <v>43</v>
-      </c>
-      <c r="C13" s="23" t="s">
-        <v>44</v>
       </c>
       <c r="D13" s="23">
         <v>1</v>
@@ -1274,18 +1274,18 @@
         <v>1.72</v>
       </c>
       <c r="J13" s="25" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="14" spans="1:12">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A14" s="23" t="s">
         <v>18</v>
       </c>
       <c r="B14" s="23" t="s">
+        <v>45</v>
+      </c>
+      <c r="C14" s="23" t="s">
         <v>46</v>
-      </c>
-      <c r="C14" s="23" t="s">
-        <v>47</v>
       </c>
       <c r="D14" s="23">
         <v>1</v>
@@ -1305,18 +1305,18 @@
         <v>0.39</v>
       </c>
       <c r="J14" s="25" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="15" spans="1:12">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A15" s="23" t="s">
         <v>18</v>
       </c>
       <c r="B15" s="23" t="s">
+        <v>48</v>
+      </c>
+      <c r="C15" s="23" t="s">
         <v>49</v>
-      </c>
-      <c r="C15" s="23" t="s">
-        <v>50</v>
       </c>
       <c r="D15" s="23">
         <v>1</v>
@@ -1336,15 +1336,15 @@
         <v>0.79</v>
       </c>
       <c r="J15" s="25" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A16" s="23" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="16" spans="1:12">
-      <c r="A16" s="23" t="s">
+      <c r="B16" s="23" t="s">
         <v>52</v>
-      </c>
-      <c r="B16" s="23" t="s">
-        <v>53</v>
       </c>
       <c r="C16" s="23"/>
       <c r="D16" s="23">
@@ -1365,16 +1365,16 @@
         <v>3.15</v>
       </c>
       <c r="J16" s="25" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="K16" s="8"/>
     </row>
-    <row r="17" spans="1:13">
+    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A17" s="23" t="s">
         <v>18</v>
       </c>
       <c r="B17" s="23" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C17" s="23"/>
       <c r="D17" s="23">
@@ -1394,12 +1394,12 @@
       <c r="J17" s="31"/>
       <c r="K17" s="8"/>
     </row>
-    <row r="18" spans="1:13" ht="16.5" customHeight="1">
+    <row r="18" spans="1:13" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="23" t="s">
+        <v>55</v>
+      </c>
+      <c r="B18" s="23" t="s">
         <v>56</v>
-      </c>
-      <c r="B18" s="23" t="s">
-        <v>57</v>
       </c>
       <c r="C18" s="23"/>
       <c r="D18" s="23">
@@ -1417,19 +1417,19 @@
       </c>
       <c r="H18" s="32"/>
     </row>
-    <row r="19" spans="1:13" ht="16.5" customHeight="1" thickBot="1">
+    <row r="19" spans="1:13" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="F19" s="29"/>
       <c r="G19" s="18"/>
       <c r="H19" s="18"/>
     </row>
-    <row r="20" spans="1:13" ht="16.5" thickBot="1">
+    <row r="20" spans="1:13" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="14" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A21" s="15" t="s">
         <v>58</v>
-      </c>
-    </row>
-    <row r="21" spans="1:13">
-      <c r="A21" s="15" t="s">
-        <v>59</v>
       </c>
       <c r="B21" s="15" t="s">
         <v>8</v>
@@ -1457,15 +1457,15 @@
         <v>16</v>
       </c>
     </row>
-    <row r="22" spans="1:13">
+    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A22" s="23" t="s">
         <v>18</v>
       </c>
       <c r="B22" s="23" t="s">
+        <v>59</v>
+      </c>
+      <c r="C22" s="23" t="s">
         <v>60</v>
-      </c>
-      <c r="C22" s="23" t="s">
-        <v>61</v>
       </c>
       <c r="D22" s="23">
         <v>1</v>
@@ -1487,12 +1487,12 @@
       <c r="J22" s="25"/>
       <c r="K22" s="8"/>
     </row>
-    <row r="23" spans="1:13">
+    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A23" s="23" t="s">
+        <v>61</v>
+      </c>
+      <c r="B23" s="23" t="s">
         <v>62</v>
-      </c>
-      <c r="B23" s="23" t="s">
-        <v>63</v>
       </c>
       <c r="C23" s="23"/>
       <c r="D23" s="23">
@@ -1515,16 +1515,16 @@
       <c r="J23" s="31"/>
       <c r="K23" s="8"/>
     </row>
-    <row r="24" spans="1:13" ht="15.75" thickBot="1">
+    <row r="24" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="F24" s="29"/>
       <c r="G24" s="29"/>
       <c r="H24" s="30"/>
       <c r="J24" s="31"/>
       <c r="K24" s="8"/>
     </row>
-    <row r="25" spans="1:13" ht="15.75" thickBot="1">
+    <row r="25" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A25" s="21" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B25" s="27">
         <v>25</v>
@@ -1535,33 +1535,33 @@
       <c r="H25" s="19"/>
       <c r="M25" s="8"/>
     </row>
-    <row r="26" spans="1:13">
+    <row r="26" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A26" s="15" t="s">
+        <v>64</v>
+      </c>
+      <c r="B26" s="33" t="s">
         <v>65</v>
-      </c>
-      <c r="B26" s="33" t="s">
-        <v>66</v>
       </c>
       <c r="C26" s="15"/>
       <c r="D26" s="15" t="s">
         <v>10</v>
       </c>
       <c r="E26" s="15" t="s">
+        <v>66</v>
+      </c>
+      <c r="F26" s="15" t="s">
         <v>67</v>
       </c>
-      <c r="F26" s="15" t="s">
+      <c r="G26" s="15" t="s">
         <v>68</v>
-      </c>
-      <c r="G26" s="15" t="s">
-        <v>69</v>
       </c>
       <c r="H26" s="15" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="27" spans="1:13">
+    <row r="27" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A27" s="23" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B27" s="23"/>
       <c r="C27" s="23"/>
@@ -1580,9 +1580,9 @@
       </c>
       <c r="H27" s="25"/>
     </row>
-    <row r="28" spans="1:13">
+    <row r="28" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A28" s="23" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B28" s="23"/>
       <c r="C28" s="23"/>
@@ -1601,9 +1601,9 @@
       </c>
       <c r="H28" s="25"/>
     </row>
-    <row r="29" spans="1:13">
+    <row r="29" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A29" s="23" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B29" s="23"/>
       <c r="C29" s="23"/>
@@ -1622,9 +1622,9 @@
       </c>
       <c r="H29" s="25"/>
     </row>
-    <row r="30" spans="1:13">
+    <row r="30" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A30" s="23" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B30" s="23"/>
       <c r="C30" s="23"/>
@@ -1643,9 +1643,9 @@
       </c>
       <c r="H30" s="25"/>
     </row>
-    <row r="31" spans="1:13">
+    <row r="31" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A31" s="23" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B31" s="23"/>
       <c r="C31" s="23"/>
@@ -1664,10 +1664,10 @@
       </c>
       <c r="H31" s="25"/>
     </row>
-    <row r="32" spans="1:13" ht="15.75" thickBot="1">
+    <row r="32" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A32" s="11"/>
       <c r="E32" s="34" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="F32" s="35">
         <f>SUM(F27:F31)</f>
@@ -1675,9 +1675,9 @@
       </c>
       <c r="H32" s="12"/>
     </row>
-    <row r="33" spans="1:13" ht="15.75" thickBot="1">
+    <row r="33" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A33" s="22" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B33" s="10"/>
       <c r="C33" s="10"/>
@@ -1692,20 +1692,20 @@
       <c r="L33" s="10"/>
       <c r="M33" s="10"/>
     </row>
-    <row r="34" spans="1:13">
+    <row r="34" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A34" s="23" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="35" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A35" s="23" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="35" spans="1:13">
-      <c r="A35" s="23" t="s">
+    <row r="39" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="40" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A40" s="22" t="s">
         <v>78</v>
-      </c>
-    </row>
-    <row r="39" spans="1:13" ht="15.75" thickBot="1"/>
-    <row r="40" spans="1:13" ht="15.75" thickBot="1">
-      <c r="A40" s="22" t="s">
-        <v>79</v>
       </c>
       <c r="B40" s="26"/>
       <c r="C40" s="10"/>
@@ -1720,29 +1720,29 @@
       <c r="L40" s="10"/>
       <c r="M40" s="10"/>
     </row>
-    <row r="41" spans="1:13">
+    <row r="41" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A41" s="37" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B41" s="37" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="42" spans="1:13">
+    <row r="42" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A42" s="23" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B42" s="25" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="43" spans="1:13">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="43" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B43" s="31"/>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="J5" r:id="rId1" xr:uid="{0946BC76-D210-43C1-94AC-7D848F3777E8}"/>
-    <hyperlink ref="J10" r:id="rId2" xr:uid="{EA254EE7-AEEF-4A0B-A8F2-28896C1DE9D5}"/>
+    <hyperlink ref="J10" r:id="rId2" display=" " xr:uid="{EA254EE7-AEEF-4A0B-A8F2-28896C1DE9D5}"/>
     <hyperlink ref="J8" r:id="rId3" xr:uid="{B80F4698-18CB-4DC3-96CF-AF1C0570978B}"/>
     <hyperlink ref="J9" r:id="rId4" xr:uid="{3BED90AA-9BDC-46BA-8B22-09F7C457779A}"/>
     <hyperlink ref="J14" r:id="rId5" xr:uid="{67933142-47EC-4E12-BFB3-314EA6B2D99A}"/>
@@ -1761,6 +1761,26 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="cf9f6c1f-8ad0-4eb8-bb2b-fb0b622a341e">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="72c39c84-b0a3-45a2-a38c-ff46bb47f11f" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100B51EC7ECFAC78D4E8EF6CBAFFF0B3505" ma:contentTypeVersion="16" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="a38268523a36e7284a4a2063ac01106c">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="cf9f6c1f-8ad0-4eb8-bb2b-fb0b622a341e" xmlns:ns3="72c39c84-b0a3-45a2-a38c-ff46bb47f11f" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="890835d1009e2f2eb5b198bf07e33774" ns2:_="" ns3:_="">
     <xsd:import namespace="cf9f6c1f-8ad0-4eb8-bb2b-fb0b622a341e"/>
@@ -1997,34 +2017,40 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="cf9f6c1f-8ad0-4eb8-bb2b-fb0b622a341e">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="72c39c84-b0a3-45a2-a38c-ff46bb47f11f" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5AB2BBFF-090D-40DF-B5CC-B4F2201C74D9}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E4958292-C6C4-482B-887A-6CF9FB19AB74}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="cf9f6c1f-8ad0-4eb8-bb2b-fb0b622a341e"/>
+    <ds:schemaRef ds:uri="72c39c84-b0a3-45a2-a38c-ff46bb47f11f"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4740145F-09D2-466B-B9A2-2798696B0ADF}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4740145F-09D2-466B-B9A2-2798696B0ADF}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E4958292-C6C4-482B-887A-6CF9FB19AB74}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5AB2BBFF-090D-40DF-B5CC-B4F2201C74D9}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="cf9f6c1f-8ad0-4eb8-bb2b-fb0b622a341e"/>
+    <ds:schemaRef ds:uri="72c39c84-b0a3-45a2-a38c-ff46bb47f11f"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>